<commit_message>
fix TN subplot moose classification
</commit_message>
<xml_diff>
--- a/final carbon data/env_subplots_final.xlsx
+++ b/final carbon data/env_subplots_final.xlsx
@@ -5773,7 +5773,9 @@
       <c r="R50" t="n">
         <v>32</v>
       </c>
-      <c r="S50"/>
+      <c r="S50" t="n">
+        <v>2</v>
+      </c>
       <c r="T50" t="n">
         <v>106</v>
       </c>
@@ -5833,7 +5835,9 @@
       <c r="R51" t="n">
         <v>32</v>
       </c>
-      <c r="S51"/>
+      <c r="S51" t="n">
+        <v>2</v>
+      </c>
       <c r="T51" t="n">
         <v>181</v>
       </c>
@@ -5893,7 +5897,9 @@
       <c r="R52" t="n">
         <v>32</v>
       </c>
-      <c r="S52"/>
+      <c r="S52" t="n">
+        <v>2</v>
+      </c>
       <c r="T52" t="n">
         <v>181</v>
       </c>
@@ -5953,7 +5959,9 @@
       <c r="R53" t="n">
         <v>32</v>
       </c>
-      <c r="S53"/>
+      <c r="S53" t="n">
+        <v>2</v>
+      </c>
       <c r="T53" t="n">
         <v>106</v>
       </c>
@@ -6013,9 +6021,7 @@
       <c r="R54" t="n">
         <v>44</v>
       </c>
-      <c r="S54" t="n">
-        <v>4</v>
-      </c>
+      <c r="S54"/>
       <c r="T54" t="n">
         <v>91</v>
       </c>
@@ -6075,9 +6081,7 @@
       <c r="R55" t="n">
         <v>44</v>
       </c>
-      <c r="S55" t="n">
-        <v>4</v>
-      </c>
+      <c r="S55"/>
       <c r="T55" t="n">
         <v>91</v>
       </c>
@@ -6137,9 +6141,7 @@
       <c r="R56" t="n">
         <v>30</v>
       </c>
-      <c r="S56" t="n">
-        <v>4</v>
-      </c>
+      <c r="S56"/>
       <c r="T56" t="n">
         <v>91</v>
       </c>
@@ -6199,9 +6201,7 @@
       <c r="R57" t="n">
         <v>30</v>
       </c>
-      <c r="S57" t="n">
-        <v>4</v>
-      </c>
+      <c r="S57"/>
       <c r="T57" t="n">
         <v>91</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>64</v>
       </c>
       <c r="S70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T70" t="n">
         <v>104</v>
@@ -7068,7 +7068,7 @@
         <v>64</v>
       </c>
       <c r="S71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T71" t="n">
         <v>93</v>
@@ -7130,7 +7130,7 @@
         <v>64</v>
       </c>
       <c r="S72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T72" t="n">
         <v>104</v>
@@ -7192,7 +7192,7 @@
         <v>52</v>
       </c>
       <c r="S73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T73" t="n">
         <v>104</v>
@@ -7502,7 +7502,7 @@
         <v>56</v>
       </c>
       <c r="S78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T78" t="n">
         <v>98</v>
@@ -7564,7 +7564,7 @@
         <v>56</v>
       </c>
       <c r="S79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T79" t="n">
         <v>100</v>
@@ -7626,7 +7626,7 @@
         <v>56</v>
       </c>
       <c r="S80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T80" t="n">
         <v>98</v>
@@ -7688,7 +7688,7 @@
         <v>45</v>
       </c>
       <c r="S81" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T81" t="n">
         <v>98</v>
@@ -7750,7 +7750,7 @@
         <v>23</v>
       </c>
       <c r="S82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T82" t="n">
         <v>79</v>
@@ -7812,7 +7812,7 @@
         <v>23</v>
       </c>
       <c r="S83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T83" t="n">
         <v>81</v>
@@ -7874,7 +7874,7 @@
         <v>23</v>
       </c>
       <c r="S84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T84" t="n">
         <v>81</v>
@@ -7936,7 +7936,7 @@
         <v>23</v>
       </c>
       <c r="S85" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T85" t="n">
         <v>81</v>
@@ -8246,7 +8246,7 @@
         <v>66</v>
       </c>
       <c r="S90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T90" t="n">
         <v>152</v>
@@ -8308,7 +8308,7 @@
         <v>66</v>
       </c>
       <c r="S91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T91" t="n">
         <v>145</v>
@@ -8370,7 +8370,7 @@
         <v>66</v>
       </c>
       <c r="S92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T92" t="n">
         <v>152</v>
@@ -8432,7 +8432,7 @@
         <v>66</v>
       </c>
       <c r="S93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T93" t="n">
         <v>152</v>
@@ -8738,7 +8738,7 @@
         <v>18</v>
       </c>
       <c r="S98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T98" t="n">
         <v>145</v>
@@ -8796,7 +8796,7 @@
         <v>14</v>
       </c>
       <c r="S99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T99" t="n">
         <v>145</v>
@@ -8854,7 +8854,7 @@
         <v>14</v>
       </c>
       <c r="S100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T100" t="n">
         <v>145</v>
@@ -8912,7 +8912,7 @@
         <v>14</v>
       </c>
       <c r="S101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T101" t="n">
         <v>145</v>
@@ -9468,7 +9468,7 @@
         <v>22</v>
       </c>
       <c r="S110" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T110" t="n">
         <v>188</v>
@@ -9528,7 +9528,7 @@
         <v>34</v>
       </c>
       <c r="S111" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T111" t="n">
         <v>177</v>
@@ -9588,7 +9588,7 @@
         <v>34</v>
       </c>
       <c r="S112" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T112" t="n">
         <v>177</v>
@@ -9648,7 +9648,7 @@
         <v>34</v>
       </c>
       <c r="S113" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T113" t="n">
         <v>177</v>
@@ -10268,7 +10268,7 @@
         <v>35</v>
       </c>
       <c r="S123" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T123" t="n">
         <v>97</v>
@@ -10330,7 +10330,7 @@
         <v>24</v>
       </c>
       <c r="S124" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T124" t="n">
         <v>97</v>
@@ -10392,7 +10392,7 @@
         <v>9</v>
       </c>
       <c r="S125" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T125" t="n">
         <v>96</v>
@@ -10454,7 +10454,7 @@
         <v>15</v>
       </c>
       <c r="S126" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T126" t="n">
         <v>97</v>
@@ -10516,7 +10516,7 @@
         <v>26</v>
       </c>
       <c r="S127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T127" t="n">
         <v>180</v>
@@ -10578,7 +10578,7 @@
         <v>29</v>
       </c>
       <c r="S128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T128" t="n">
         <v>170</v>
@@ -10640,7 +10640,7 @@
         <v>26</v>
       </c>
       <c r="S129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T129" t="n">
         <v>179</v>
@@ -10702,7 +10702,7 @@
         <v>22</v>
       </c>
       <c r="S130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T130" t="n">
         <v>182</v>
@@ -11198,7 +11198,7 @@
         <v>33</v>
       </c>
       <c r="S138" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T138" t="n">
         <v>95</v>
@@ -11260,7 +11260,7 @@
         <v>30</v>
       </c>
       <c r="S139" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T139" t="n">
         <v>95</v>
@@ -11322,7 +11322,7 @@
         <v>33</v>
       </c>
       <c r="S140" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T140" t="n">
         <v>95</v>
@@ -11384,7 +11384,7 @@
         <v>30</v>
       </c>
       <c r="S141" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T141" t="n">
         <v>91</v>

</xml_diff>

<commit_message>
think actually set TN 05 this time
</commit_message>
<xml_diff>
--- a/final carbon data/env_subplots_final.xlsx
+++ b/final carbon data/env_subplots_final.xlsx
@@ -6021,7 +6021,9 @@
       <c r="R54" t="n">
         <v>44</v>
       </c>
-      <c r="S54"/>
+      <c r="S54" t="n">
+        <v>2</v>
+      </c>
       <c r="T54" t="n">
         <v>91</v>
       </c>
@@ -6081,7 +6083,9 @@
       <c r="R55" t="n">
         <v>44</v>
       </c>
-      <c r="S55"/>
+      <c r="S55" t="n">
+        <v>2</v>
+      </c>
       <c r="T55" t="n">
         <v>91</v>
       </c>
@@ -6141,7 +6145,9 @@
       <c r="R56" t="n">
         <v>30</v>
       </c>
-      <c r="S56"/>
+      <c r="S56" t="n">
+        <v>2</v>
+      </c>
       <c r="T56" t="n">
         <v>91</v>
       </c>
@@ -6201,7 +6207,9 @@
       <c r="R57" t="n">
         <v>30</v>
       </c>
-      <c r="S57"/>
+      <c r="S57" t="n">
+        <v>2</v>
+      </c>
       <c r="T57" t="n">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
forgot actually want to set initial moose level to one so it get converted to 3 (H)
</commit_message>
<xml_diff>
--- a/final carbon data/env_subplots_final.xlsx
+++ b/final carbon data/env_subplots_final.xlsx
@@ -6022,7 +6022,7 @@
         <v>44</v>
       </c>
       <c r="S54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T54" t="n">
         <v>91</v>
@@ -6084,7 +6084,7 @@
         <v>44</v>
       </c>
       <c r="S55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T55" t="n">
         <v>91</v>
@@ -6146,7 +6146,7 @@
         <v>30</v>
       </c>
       <c r="S56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T56" t="n">
         <v>91</v>
@@ -6208,7 +6208,7 @@
         <v>30</v>
       </c>
       <c r="S57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T57" t="n">
         <v>91</v>

</xml_diff>

<commit_message>
forgot to fix NA aspects for subplot levels
</commit_message>
<xml_diff>
--- a/final carbon data/env_subplots_final.xlsx
+++ b/final carbon data/env_subplots_final.xlsx
@@ -8961,7 +8961,9 @@
       <c r="N102" t="n">
         <v>110</v>
       </c>
-      <c r="O102"/>
+      <c r="O102" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P102" t="n">
         <v>4512</v>
       </c>
@@ -9517,7 +9519,9 @@
       <c r="N111" t="n">
         <v>123</v>
       </c>
-      <c r="O111"/>
+      <c r="O111" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P111" t="n">
         <v>2582</v>
       </c>
@@ -9577,7 +9581,9 @@
       <c r="N112" t="n">
         <v>123</v>
       </c>
-      <c r="O112"/>
+      <c r="O112" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P112" t="n">
         <v>2582</v>
       </c>
@@ -9637,7 +9643,9 @@
       <c r="N113" t="n">
         <v>123</v>
       </c>
-      <c r="O113"/>
+      <c r="O113" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P113" t="n">
         <v>2582</v>
       </c>
@@ -16641,7 +16649,9 @@
       <c r="N226" t="n">
         <v>16</v>
       </c>
-      <c r="O226"/>
+      <c r="O226" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P226" t="n">
         <v>3627</v>
       </c>
@@ -16701,7 +16711,9 @@
       <c r="N227" t="n">
         <v>16</v>
       </c>
-      <c r="O227"/>
+      <c r="O227" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P227" t="n">
         <v>3638</v>
       </c>
@@ -16761,7 +16773,9 @@
       <c r="N228" t="n">
         <v>16</v>
       </c>
-      <c r="O228"/>
+      <c r="O228" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P228" t="n">
         <v>3638</v>
       </c>
@@ -16821,7 +16835,9 @@
       <c r="N229" t="n">
         <v>16</v>
       </c>
-      <c r="O229"/>
+      <c r="O229" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P229" t="n">
         <v>3627</v>
       </c>
@@ -20353,7 +20369,9 @@
       <c r="N286" t="n">
         <v>60</v>
       </c>
-      <c r="O286"/>
+      <c r="O286" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P286" t="n">
         <v>4083</v>
       </c>
@@ -20413,7 +20431,9 @@
       <c r="N287" t="n">
         <v>60</v>
       </c>
-      <c r="O287"/>
+      <c r="O287" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P287" t="n">
         <v>4191</v>
       </c>
@@ -20473,7 +20493,9 @@
       <c r="N288" t="n">
         <v>60</v>
       </c>
-      <c r="O288"/>
+      <c r="O288" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P288" t="n">
         <v>4083</v>
       </c>
@@ -23819,7 +23841,9 @@
       <c r="N342" t="n">
         <v>21</v>
       </c>
-      <c r="O342"/>
+      <c r="O342" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P342" t="n">
         <v>3653</v>
       </c>
@@ -24003,7 +24027,9 @@
       <c r="N345" t="n">
         <v>21</v>
       </c>
-      <c r="O345"/>
+      <c r="O345" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P345" t="n">
         <v>3653</v>
       </c>

</xml_diff>